<commit_message>
log transactions to the correct mongo collection
</commit_message>
<xml_diff>
--- a/templates/main_template.xlsx
+++ b/templates/main_template.xlsx
@@ -49,7 +49,7 @@
     <t>Unkown</t>
   </si>
   <si>
-    <t>{unkown}</t>
+    <t>{unknown}</t>
   </si>
   <si>
     <t>Groceries/Snacks</t>
@@ -142,7 +142,7 @@
     <t>Electric</t>
   </si>
   <si>
-    <t/>
+    <t>{electricity}</t>
   </si>
   <si>
     <t>{other_living_expenses}</t>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -205,9 +205,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -523,14 +520,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="65.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="65.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -741,7 +738,7 @@
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="1"/>

</xml_diff>